<commit_message>
second commit by ajmal
</commit_message>
<xml_diff>
--- a/chromeOutput.xlsx
+++ b/chromeOutput.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5410" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5618" uniqueCount="104">
   <si>
     <t>COURSE NAME</t>
   </si>
@@ -49,67 +49,67 @@
     <t>English</t>
   </si>
   <si>
-    <t>1200</t>
+    <t>1203</t>
   </si>
   <si>
     <t>Spanish</t>
   </si>
   <si>
-    <t>472</t>
+    <t>488</t>
   </si>
   <si>
     <t>Russian</t>
   </si>
   <si>
-    <t>403</t>
+    <t>421</t>
   </si>
   <si>
     <t>French</t>
   </si>
   <si>
-    <t>372</t>
+    <t>390</t>
   </si>
   <si>
     <t>Portuguese</t>
   </si>
   <si>
-    <t>283</t>
+    <t>312</t>
   </si>
   <si>
     <t>Arabic</t>
   </si>
   <si>
-    <t>148</t>
+    <t>171</t>
   </si>
   <si>
     <t>Chinese (China)</t>
   </si>
   <si>
-    <t>139</t>
+    <t>137</t>
   </si>
   <si>
     <t>Korean</t>
   </si>
   <si>
+    <t>German</t>
+  </si>
+  <si>
     <t>110</t>
   </si>
   <si>
     <t>Vietnamese</t>
   </si>
   <si>
-    <t>87</t>
-  </si>
-  <si>
-    <t>German</t>
-  </si>
-  <si>
-    <t>85</t>
-  </si>
-  <si>
     <t>Portuguese (Brazil)</t>
   </si>
   <si>
-    <t>75</t>
+    <t>73</t>
+  </si>
+  <si>
+    <t>Turkish</t>
+  </si>
+  <si>
+    <t>70</t>
   </si>
   <si>
     <t>Japanese</t>
@@ -118,10 +118,10 @@
     <t>67</t>
   </si>
   <si>
-    <t>Turkish</t>
-  </si>
-  <si>
-    <t>46</t>
+    <t>Italian</t>
+  </si>
+  <si>
+    <t>45</t>
   </si>
   <si>
     <t>Persian</t>
@@ -133,87 +133,93 @@
     <t>Chinese (Traditional)</t>
   </si>
   <si>
-    <t>34</t>
+    <t>31</t>
+  </si>
+  <si>
+    <t>Chinese</t>
+  </si>
+  <si>
+    <t>30</t>
   </si>
   <si>
     <t>Greek</t>
   </si>
   <si>
-    <t>24</t>
+    <t>25</t>
   </si>
   <si>
     <t>Ukrainian</t>
   </si>
   <si>
-    <t>23</t>
+    <t>22</t>
   </si>
   <si>
     <t>Hindi</t>
   </si>
   <si>
-    <t>19</t>
+    <t>20</t>
   </si>
   <si>
     <t>Romanian</t>
   </si>
   <si>
-    <t>15</t>
+    <t>16</t>
+  </si>
+  <si>
+    <t>Hebrew</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>Catalan</t>
+  </si>
+  <si>
+    <t>11</t>
   </si>
   <si>
     <t>Dutch</t>
   </si>
   <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>Italian</t>
-  </si>
-  <si>
-    <t>Catalan</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>Hebrew</t>
+    <t>10</t>
   </si>
   <si>
     <t>Thai</t>
   </si>
   <si>
-    <t>11</t>
+    <t>9</t>
+  </si>
+  <si>
+    <t>Polish</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Afrikaans</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Mongolian</t>
+  </si>
+  <si>
+    <t>Serbian</t>
   </si>
   <si>
     <t>Indonesian</t>
   </si>
   <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>Polish</t>
-  </si>
-  <si>
-    <t>Afrikaans</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>Mongolian</t>
+    <t>6</t>
   </si>
   <si>
     <t>Portuguese (Portugal)</t>
   </si>
   <si>
-    <t>Serbian</t>
-  </si>
-  <si>
     <t>Tamil</t>
   </si>
   <si>
-    <t>6</t>
-  </si>
-  <si>
     <t>Hungarian</t>
   </si>
   <si>
@@ -235,36 +241,36 @@
     <t>Telugu</t>
   </si>
   <si>
+    <t>Urdu</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Albanian</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Bulgarian</t>
+  </si>
+  <si>
+    <t>Burmese</t>
+  </si>
+  <si>
+    <t>Estonian</t>
+  </si>
+  <si>
+    <t>Georgian</t>
+  </si>
+  <si>
+    <t>Kazakh</t>
+  </si>
+  <si>
     <t>Lithuanian</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>Urdu</t>
-  </si>
-  <si>
-    <t>Albanian</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>Bulgarian</t>
-  </si>
-  <si>
-    <t>Burmese</t>
-  </si>
-  <si>
-    <t>Estonian</t>
-  </si>
-  <si>
-    <t>Georgian</t>
-  </si>
-  <si>
-    <t>Kazakh</t>
-  </si>
-  <si>
     <t>Uzbek</t>
   </si>
   <si>
@@ -286,7 +292,7 @@
     <t>TOTAL COURSES</t>
   </si>
   <si>
-    <t>3794</t>
+    <t>4048</t>
   </si>
   <si>
     <t>LEVEL NAME</t>
@@ -298,25 +304,25 @@
     <t>Intermediate</t>
   </si>
   <si>
-    <t>528</t>
+    <t>530</t>
   </si>
   <si>
     <t>Beginner</t>
   </si>
   <si>
-    <t>500</t>
+    <t>492</t>
   </si>
   <si>
     <t>Mixed</t>
   </si>
   <si>
-    <t>233</t>
+    <t>230</t>
   </si>
   <si>
     <t>Advanced</t>
   </si>
   <si>
-    <t>69</t>
+    <t>78</t>
   </si>
   <si>
     <t>1330</t>
@@ -415,7 +421,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B51"/>
+  <dimension ref="A1:B52"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -494,108 +500,108 @@
         <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
         <v>26</v>
-      </c>
-      <c r="B10" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B16" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B20" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B21" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B22" t="s">
         <v>49</v>
@@ -603,18 +609,18 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" t="s">
         <v>51</v>
-      </c>
-      <c r="B23" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" t="s">
         <v>53</v>
-      </c>
-      <c r="B24" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="25">
@@ -638,44 +644,44 @@
         <v>58</v>
       </c>
       <c r="B27" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B28" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29" t="s">
         <v>61</v>
-      </c>
-      <c r="B29" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B30" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B31" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B32" t="s">
         <v>65</v>
@@ -683,10 +689,10 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B33" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34">
@@ -694,15 +700,15 @@
         <v>68</v>
       </c>
       <c r="B34" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
+        <v>70</v>
+      </c>
+      <c r="B35" t="s">
         <v>69</v>
-      </c>
-      <c r="B35" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="36">
@@ -710,23 +716,23 @@
         <v>71</v>
       </c>
       <c r="B36" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
+        <v>73</v>
+      </c>
+      <c r="B37" t="s">
         <v>72</v>
-      </c>
-      <c r="B37" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B38" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="39">
@@ -734,71 +740,71 @@
         <v>75</v>
       </c>
       <c r="B39" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B40" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
+        <v>79</v>
+      </c>
+      <c r="B41" t="s">
         <v>78</v>
-      </c>
-      <c r="B41" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B42" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B43" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B44" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B45" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B46" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B47" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="48">
@@ -806,31 +812,39 @@
         <v>86</v>
       </c>
       <c r="B48" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
+        <v>88</v>
+      </c>
+      <c r="B49" t="s">
         <v>87</v>
-      </c>
-      <c r="B49" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B50" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B51" t="s">
-        <v>90</v>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>91</v>
+      </c>
+      <c r="B52" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -852,50 +866,50 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B3" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B5" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B6" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
third commit by ajmal
</commit_message>
<xml_diff>
--- a/chromeOutput.xlsx
+++ b/chromeOutput.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5618" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5618" uniqueCount="105">
   <si>
     <t>COURSE NAME</t>
   </si>
@@ -49,99 +49,105 @@
     <t>English</t>
   </si>
   <si>
-    <t>1203</t>
+    <t>1207</t>
   </si>
   <si>
     <t>Spanish</t>
   </si>
   <si>
-    <t>488</t>
+    <t>491</t>
   </si>
   <si>
     <t>Russian</t>
   </si>
   <si>
-    <t>421</t>
+    <t>426</t>
   </si>
   <si>
     <t>French</t>
   </si>
   <si>
-    <t>390</t>
+    <t>395</t>
   </si>
   <si>
     <t>Portuguese</t>
   </si>
   <si>
-    <t>312</t>
+    <t>320</t>
   </si>
   <si>
     <t>Arabic</t>
   </si>
   <si>
-    <t>171</t>
+    <t>186</t>
+  </si>
+  <si>
+    <t>Korean</t>
+  </si>
+  <si>
+    <t>146</t>
   </si>
   <si>
     <t>Chinese (China)</t>
   </si>
   <si>
-    <t>137</t>
-  </si>
-  <si>
-    <t>Korean</t>
+    <t>138</t>
   </si>
   <si>
     <t>German</t>
   </si>
   <si>
-    <t>110</t>
+    <t>124</t>
   </si>
   <si>
     <t>Vietnamese</t>
   </si>
   <si>
+    <t>121</t>
+  </si>
+  <si>
+    <t>Turkish</t>
+  </si>
+  <si>
+    <t>86</t>
+  </si>
+  <si>
     <t>Portuguese (Brazil)</t>
   </si>
   <si>
-    <t>73</t>
-  </si>
-  <si>
-    <t>Turkish</t>
-  </si>
-  <si>
-    <t>70</t>
+    <t>76</t>
   </si>
   <si>
     <t>Japanese</t>
   </si>
   <si>
-    <t>67</t>
+    <t>68</t>
   </si>
   <si>
     <t>Italian</t>
   </si>
   <si>
-    <t>45</t>
+    <t>56</t>
+  </si>
+  <si>
+    <t>Chinese</t>
+  </si>
+  <si>
+    <t>41</t>
   </si>
   <si>
     <t>Persian</t>
   </si>
   <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>Chinese (Traditional)</t>
+  </si>
+  <si>
     <t>35</t>
   </si>
   <si>
-    <t>Chinese (Traditional)</t>
-  </si>
-  <si>
-    <t>31</t>
-  </si>
-  <si>
-    <t>Chinese</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
     <t>Greek</t>
   </si>
   <si>
@@ -163,7 +169,7 @@
     <t>Romanian</t>
   </si>
   <si>
-    <t>16</t>
+    <t>14</t>
   </si>
   <si>
     <t>Hebrew</t>
@@ -172,30 +178,30 @@
     <t>13</t>
   </si>
   <si>
+    <t>Dutch</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
     <t>Catalan</t>
   </si>
   <si>
     <t>11</t>
   </si>
   <si>
-    <t>Dutch</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
     <t>Thai</t>
   </si>
   <si>
-    <t>9</t>
+    <t>Indonesian</t>
+  </si>
+  <si>
+    <t>8</t>
   </si>
   <si>
     <t>Polish</t>
   </si>
   <si>
-    <t>8</t>
-  </si>
-  <si>
     <t>Afrikaans</t>
   </si>
   <si>
@@ -205,39 +211,36 @@
     <t>Mongolian</t>
   </si>
   <si>
+    <t>Portuguese (Portugal)</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
     <t>Serbian</t>
   </si>
   <si>
-    <t>Indonesian</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>Portuguese (Portugal)</t>
-  </si>
-  <si>
     <t>Tamil</t>
   </si>
   <si>
+    <t>Slovak</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Bengali</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Czech</t>
+  </si>
+  <si>
     <t>Hungarian</t>
   </si>
   <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>Slovak</t>
-  </si>
-  <si>
-    <t>Bengali</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>Czech</t>
-  </si>
-  <si>
     <t>Telugu</t>
   </si>
   <si>
@@ -292,7 +295,7 @@
     <t>TOTAL COURSES</t>
   </si>
   <si>
-    <t>4048</t>
+    <t>4172</t>
   </si>
   <si>
     <t>LEVEL NAME</t>
@@ -304,28 +307,28 @@
     <t>Intermediate</t>
   </si>
   <si>
-    <t>530</t>
+    <t>538</t>
   </si>
   <si>
     <t>Beginner</t>
   </si>
   <si>
-    <t>492</t>
+    <t>502</t>
   </si>
   <si>
     <t>Mixed</t>
   </si>
   <si>
-    <t>230</t>
+    <t>222</t>
   </si>
   <si>
     <t>Advanced</t>
   </si>
   <si>
-    <t>78</t>
-  </si>
-  <si>
-    <t>1330</t>
+    <t>74</t>
+  </si>
+  <si>
+    <t>1336</t>
   </si>
 </sst>
 </file>
@@ -500,140 +503,140 @@
         <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B21" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B22" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B23" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B24" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B25" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B26" t="s">
         <v>57</v>
@@ -641,18 +644,18 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B27" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
+        <v>61</v>
+      </c>
+      <c r="B28" t="s">
         <v>60</v>
-      </c>
-      <c r="B28" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="29">
@@ -660,60 +663,60 @@
         <v>62</v>
       </c>
       <c r="B29" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30" t="s">
         <v>63</v>
-      </c>
-      <c r="B30" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B31" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
+        <v>67</v>
+      </c>
+      <c r="B32" t="s">
         <v>66</v>
-      </c>
-      <c r="B32" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B33" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B34" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B35" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B36" t="s">
         <v>72</v>
@@ -721,7 +724,7 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B37" t="s">
         <v>72</v>
@@ -729,7 +732,7 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B38" t="s">
         <v>72</v>
@@ -737,114 +740,114 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B39" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B40" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
+        <v>80</v>
+      </c>
+      <c r="B41" t="s">
         <v>79</v>
-      </c>
-      <c r="B41" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B42" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B43" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B44" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B45" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B46" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B47" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B48" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
+        <v>89</v>
+      </c>
+      <c r="B49" t="s">
         <v>88</v>
-      </c>
-      <c r="B49" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B50" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B51" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B52" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -866,50 +869,50 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B6" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>